<commit_message>
udpate source and document
</commit_message>
<xml_diff>
--- a/documents/felicette_server.xlsx
+++ b/documents/felicette_server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\felicette\felicette_server\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606AC05F-BFA7-4A0C-AC04-380BF667B9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84953868-747B-410F-8C02-5FCADE38F3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
   <si>
     <t>API</t>
   </si>
@@ -103,9 +103,6 @@
     <t>sigin</t>
   </si>
   <si>
-    <t>/api/auth/signin</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t>image</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Allow CORS: Access-Control-Allow-Origin</t>
@@ -439,12 +433,277 @@
       <t>:</t>
     </r>
   </si>
+  <si>
+    <t>sigup</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"username"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"123"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"qwer@adsf.qwer"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"password"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"123"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"roles"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF098658"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"username"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"username"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"password"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>"123"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{{base_url}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF212121"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/api/auth/signup</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>{{base_url}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF212121"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>/api/auth/signin</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,6 +748,42 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFA31515"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0451A5"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF098658"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -577,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -609,15 +904,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -630,6 +916,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,50 +949,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>192441</xdr:colOff>
-      <xdr:row>90</xdr:row>
-      <xdr:rowOff>105747</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="857250" y="4457700"/>
-          <a:ext cx="13908441" cy="6963747"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -720,7 +976,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -729,6 +985,180 @@
         <a:xfrm>
           <a:off x="571500" y="3886200"/>
           <a:ext cx="14403810" cy="5811061"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>188905</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>132548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11C3D323-D459-406A-9450-4466AC169802}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="571500" y="20274643"/>
+          <a:ext cx="12761905" cy="6419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>90</xdr:col>
+      <xdr:colOff>157238</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15D30ADD-B757-4DE6-963B-720433DB7379}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect l="22673" t="19917" b="13090"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13716000" y="20655643"/>
+          <a:ext cx="12158738" cy="5538107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>255357</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>84786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DF110BF-AF9D-452A-814B-23FDCCCCF6EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="11892643"/>
+          <a:ext cx="14542857" cy="7514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>93</xdr:col>
+      <xdr:colOff>24036</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>112000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46B3FB0B-6077-423F-A6F0-BA2C4BDD37F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:srcRect l="25169" t="22454"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15716250" y="13607143"/>
+          <a:ext cx="10882536" cy="5827000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2206,145 +2636,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA96"/>
+  <dimension ref="A1:AA110"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16" t="s">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
     </row>
     <row r="2" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17" t="s">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="17"/>
-      <c r="W2" s="17"/>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="17"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="21"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2369,7 +2799,7 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2399,7 +2829,7 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2632,13 +3062,68 @@
       <c r="C52" s="12"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C96" t="s">
-        <v>32</v>
+      <c r="D53" s="24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="23" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +3158,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2694,164 +3179,164 @@
   <sheetData>
     <row r="30" spans="12:18" x14ac:dyDescent="0.25">
       <c r="L30" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" t="s">
+        <v>26</v>
+      </c>
+      <c r="N30" t="s">
         <v>25</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>27</v>
       </c>
-      <c r="N30" t="s">
-        <v>26</v>
-      </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>28</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>29</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>30</v>
       </c>
-      <c r="R30" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="59" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B59" s="21" t="s">
-        <v>106</v>
+      <c r="B59" s="18" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B60" s="19"/>
+      <c r="B60" s="16"/>
     </row>
     <row r="61" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B62" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="16"/>
+    </row>
+    <row r="65" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B65" s="17" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B62" s="20" t="s">
+    <row r="66" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B66" s="17" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B63" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B64" s="19"/>
-    </row>
-    <row r="65" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B65" s="20" t="s">
+    <row r="67" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B67" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B68" s="16"/>
+    </row>
+    <row r="69" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B66" s="20" t="s">
+    <row r="70" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B67" s="21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B68" s="19"/>
-    </row>
-    <row r="69" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B69" s="20" t="s">
+    <row r="71" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="70" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B70" s="20" t="s">
+    <row r="72" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B72" s="16"/>
+    </row>
+    <row r="73" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B73" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="71" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B71" s="18" t="s">
+    <row r="74" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B74" s="17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B72" s="19"/>
-    </row>
-    <row r="73" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B73" s="20" t="s">
+    <row r="75" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B75" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B74" s="20" t="s">
+    <row r="76" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B76" s="16"/>
+    </row>
+    <row r="77" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B75" s="18" t="s">
+    <row r="78" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B78" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B76" s="19"/>
-    </row>
-    <row r="77" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B77" s="20" t="s">
+    <row r="79" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B79" s="15" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B78" s="20" t="s">
+    <row r="80" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B80" s="16"/>
+    </row>
+    <row r="81" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B81" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B79" s="18" t="s">
+    <row r="82" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B82" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B80" s="19"/>
-    </row>
-    <row r="81" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B81" s="20" t="s">
+    <row r="83" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B83" s="15" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B82" s="20" t="s">
+    <row r="84" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B84" s="16"/>
+    </row>
+    <row r="85" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B85" s="17" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="83" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B83" s="18" t="s">
+    <row r="86" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B86" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="84" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B84" s="19"/>
-    </row>
-    <row r="85" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B85" s="20" t="s">
+    <row r="87" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B87" s="15" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B86" s="20" t="s">
+    <row r="88" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B88" s="16"/>
+    </row>
+    <row r="89" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B89" s="17" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B87" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B88" s="19"/>
-    </row>
-    <row r="89" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B89" s="20" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2864,7 +3349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:B69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -2891,337 +3376,337 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -3234,7 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -3242,22 +3727,22 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chức năng order mới tạo được thiết kế của bảng order và order detail
</commit_message>
<xml_diff>
--- a/documents/felicette_server.xlsx
+++ b/documents/felicette_server.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\felicette\felicette_server\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\felicette_server\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84953868-747B-410F-8C02-5FCADE38F3D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="139">
   <si>
     <t>API</t>
   </si>
@@ -698,11 +697,80 @@
       <t>/api/auth/signin</t>
     </r>
   </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>order_detail</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>order_date</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
+  </si>
+  <si>
+    <t>delivery_address</t>
+  </si>
+  <si>
+    <t>create_at</t>
+  </si>
+  <si>
+    <t>update_at</t>
+  </si>
+  <si>
+    <t>create_by</t>
+  </si>
+  <si>
+    <t>update_by</t>
+  </si>
+  <si>
+    <t>order_creator</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>image_order</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -916,6 +984,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -925,11 +998,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2635,142 +2703,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI13" sqref="AI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
     </row>
     <row r="2" spans="1:27" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21" t="s">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="24"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="19"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
-      <c r="AA4" s="19"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
+      <c r="Y4" s="22"/>
+      <c r="Z4" s="22"/>
+      <c r="AA4" s="22"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="19"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="22"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
@@ -3062,67 +3130,67 @@
       <c r="C52" s="12"/>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="24" t="s">
+      <c r="D53" s="21" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="23" t="s">
+      <c r="D55" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="20" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="23" t="s">
+      <c r="D57" s="20" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="23" t="s">
+      <c r="D58" s="20" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="22" t="s">
+      <c r="B103" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="24" t="s">
+      <c r="C104" s="21" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C105" s="23" t="s">
+      <c r="C105" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C106" s="23" t="s">
+      <c r="C106" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C107" s="23" t="s">
+      <c r="C107" s="20" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C108" s="23" t="s">
+      <c r="C108" s="20" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C109" s="23" t="s">
+      <c r="C109" s="20" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C110" s="23" t="s">
+      <c r="C110" s="20" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3144,7 +3212,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3168,11 +3236,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B30:R89"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3346,11 +3414,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:B69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:AA69"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3366,80 +3434,180 @@
     <col min="9" max="9" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="14"/>
+    <col min="12" max="12" width="5.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="10.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="L3" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="R4" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="U4" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="W4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y4" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z4" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA4" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="L7" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="L8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="W8" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>72</v>
       </c>
@@ -3716,7 +3884,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>